<commit_message>
boosting opt, factor importance, update paper
</commit_message>
<xml_diff>
--- a/论文用表.xlsx
+++ b/论文用表.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjzjl\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjzjl\Desktop\jianzhi\Machine_Learinng_Multi_Factor_Asset_Pricing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C26EDD2-8EA7-471B-A75F-CF3D1A70D43F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2CDD10-8C3F-47FF-8EB9-B8BD0D33D219}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="4" xr2:uid="{9F8F9D38-CFFA-4718-AE12-CF49E4640044}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{9F8F9D38-CFFA-4718-AE12-CF49E4640044}"/>
   </bookViews>
   <sheets>
     <sheet name="样本分布统计" sheetId="1" r:id="rId1"/>
     <sheet name="模型loss-rolling" sheetId="2" r:id="rId2"/>
     <sheet name="模型loss-recursive" sheetId="3" r:id="rId3"/>
-    <sheet name="factor_test" sheetId="4" r:id="rId4"/>
-    <sheet name="factor_corr" sheetId="5" r:id="rId5"/>
+    <sheet name="模型factor_importance" sheetId="6" r:id="rId4"/>
+    <sheet name="factor_test" sheetId="4" r:id="rId5"/>
+    <sheet name="factor_corr" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -143,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="79">
   <si>
     <t>年份</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -358,6 +359,85 @@
   </si>
   <si>
     <t>2008-2016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>all</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OLS + H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> batch size 500 epoch 100</t>
+  </si>
+  <si>
+    <t>mean-tp2016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>all-to2016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SIZE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ROE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VOL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INVES</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ILLIQ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXTRA_TO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REVERSAL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACCRUAL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -365,6 +445,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="176" formatCode="0.000_ "/>
+    <numFmt numFmtId="177" formatCode="0.00_ "/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -452,7 +536,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -483,11 +567,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1087,10 +1197,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1311E9FE-9019-420E-9DB5-95D6F30023B2}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1360,121 +1470,95 @@
         <v>-0.22665764493747201</v>
       </c>
     </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="1">
+        <f>AVERAGE(D4:D10)</f>
+        <v>-27879.388075486757</v>
+      </c>
+    </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="1">
+        <v>-59349.581803093097</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="D13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="9" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9" t="s">
+      <c r="F15" s="9"/>
+      <c r="G15" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="1" t="s">
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="1" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="1">
-        <v>2012</v>
-      </c>
-      <c r="C15" s="1">
-        <v>2013</v>
-      </c>
-      <c r="E15" s="1">
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="F15" s="1">
-        <v>8.3448924330490303E-3</v>
-      </c>
-      <c r="G15" s="1">
-        <v>2</v>
-      </c>
-      <c r="H15" s="1">
-        <v>2</v>
-      </c>
-      <c r="I15" s="1">
-        <v>-9.1186140663979103E-3</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="1">
+        <v>5</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2012</v>
+      </c>
+      <c r="C17" s="1">
         <v>2013</v>
       </c>
-      <c r="C16" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0.12</v>
-      </c>
-      <c r="F16" s="1">
-        <v>2.97558794477004E-2</v>
-      </c>
-      <c r="G16" s="1">
-        <v>2</v>
-      </c>
-      <c r="H16" s="1">
-        <v>2</v>
-      </c>
-      <c r="I16" s="3">
-        <v>9.6769084235503997E-5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="1">
-        <v>2014</v>
-      </c>
-      <c r="C17" s="1">
-        <v>2015</v>
+      <c r="D17" s="1">
+        <v>-19760.350582373099</v>
       </c>
       <c r="E17" s="1">
-        <v>0.128</v>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="F17" s="1">
-        <v>1.5727102057089999E-2</v>
+        <v>8.3448924330490303E-3</v>
       </c>
       <c r="G17" s="1">
         <v>2</v>
@@ -1483,50 +1567,62 @@
         <v>2</v>
       </c>
       <c r="I17" s="1">
-        <v>1.9986938599584801E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+        <v>-9.1186140663979103E-3</v>
+      </c>
+      <c r="J17" s="1">
+        <v>-5.7844652556480601E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B18" s="1">
+        <v>2013</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2014</v>
+      </c>
+      <c r="D18" s="1">
+        <v>-20657.171243368499</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="F18" s="1">
+        <v>2.97558794477004E-2</v>
+      </c>
+      <c r="G18" s="1">
+        <v>2</v>
+      </c>
+      <c r="H18" s="1">
+        <v>2</v>
+      </c>
+      <c r="I18" s="3">
+        <v>9.6769084235503997E-5</v>
+      </c>
+      <c r="J18" s="1">
+        <v>-6.6674932826690403E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2014</v>
+      </c>
+      <c r="C19" s="1">
         <v>2015</v>
       </c>
-      <c r="C18" s="1">
-        <v>2016</v>
-      </c>
-      <c r="E18" s="1">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="F18" s="1">
-        <v>3.4410436870793197E-2</v>
-      </c>
-      <c r="G18" s="1">
-        <v>6</v>
-      </c>
-      <c r="H18" s="1">
-        <v>6</v>
-      </c>
-      <c r="I18" s="1">
-        <v>1.81567665372309E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="1">
-        <v>2016</v>
-      </c>
-      <c r="C19" s="1">
-        <v>2017</v>
+      <c r="D19" s="1">
+        <v>-23274.6511441357</v>
       </c>
       <c r="E19" s="1">
-        <v>9.1999999999999998E-2</v>
+        <v>0.128</v>
       </c>
       <c r="F19" s="1">
-        <v>-0.11067894901894899</v>
+        <v>1.5727102057089999E-2</v>
       </c>
       <c r="G19" s="1">
         <v>2</v>
@@ -1535,44 +1631,192 @@
         <v>2</v>
       </c>
       <c r="I19" s="1">
+        <v>1.9986938599584801E-2</v>
+      </c>
+      <c r="J19" s="1">
+        <v>-9.9180734617761293E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D20" s="1">
+        <v>-21672.252454104</v>
+      </c>
+      <c r="E20" s="1">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <v>3.4410436870793197E-2</v>
+      </c>
+      <c r="G20" s="1">
+        <v>6</v>
+      </c>
+      <c r="H20" s="1">
+        <v>6</v>
+      </c>
+      <c r="I20" s="1">
+        <v>1.81567665372309E-2</v>
+      </c>
+      <c r="J20" s="1">
+        <v>4.0015034614006399E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2017</v>
+      </c>
+      <c r="D21" s="1">
+        <v>-30317.467478304799</v>
+      </c>
+      <c r="E21" s="1">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <v>-0.11067894901894899</v>
+      </c>
+      <c r="G21" s="1">
+        <v>2</v>
+      </c>
+      <c r="H21" s="1">
+        <v>2</v>
+      </c>
+      <c r="I21" s="1">
         <v>-0.10225928270538701</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A20" s="1" t="s">
+      <c r="J21" s="1">
+        <v>-0.64751117288634796</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B22" s="1">
         <v>2017</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C22" s="1">
         <v>2018</v>
       </c>
-      <c r="E20" s="1">
+      <c r="D22" s="1">
+        <v>-58200.773730820198</v>
+      </c>
+      <c r="E22" s="1">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F22" s="1">
         <v>-0.151093702237385</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G22" s="1">
         <v>2</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H22" s="1">
         <v>2</v>
       </c>
-      <c r="I20" s="1">
+      <c r="I22" s="1">
         <v>-0.15600442262782699</v>
+      </c>
+      <c r="J22" s="1">
+        <v>-0.53299023567952497</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="1">
+        <f>AVERAGE(D17:D22)</f>
+        <v>-28980.444438851049</v>
+      </c>
+      <c r="F23" s="1">
+        <v>-2.8922390074616999E-2</v>
+      </c>
+      <c r="I23" s="1">
+        <f>AVERAGE(I17:I22)</f>
+        <v>-3.8190307529760117E-2</v>
+      </c>
+      <c r="J23" s="1">
+        <v>-0.32844090092240202</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="1">
+        <v>-59349.581803093097</v>
+      </c>
+      <c r="F24" s="1">
+        <v>-1.18064296519317E-2</v>
+      </c>
+      <c r="I24" s="1">
+        <v>-0.16172625199999999</v>
+      </c>
+      <c r="J24" s="1">
+        <v>-0.27845189999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="1">
+        <f>AVERAGE(D17:D20)</f>
+        <v>-21341.106355995325</v>
+      </c>
+      <c r="F25" s="1">
+        <f>AVERAGE(F17:F20)</f>
+        <v>2.2059577702158155E-2</v>
+      </c>
+      <c r="I25" s="1">
+        <f>AVERAGE(I17:I20)</f>
+        <v>7.2804650386633241E-3</v>
+      </c>
+      <c r="J25" s="1">
+        <f>AVERAGE(J17:J20)</f>
+        <v>-4.5921321346731478E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="1">
+        <v>-24177.896715357001</v>
+      </c>
+      <c r="F26" s="1">
+        <v>2.0584278852400901E-2</v>
+      </c>
+      <c r="I26" s="1">
+        <v>1.0317313874273501E-2</v>
+      </c>
+      <c r="J26" s="1">
+        <v>-6.7125599999999994E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:I2"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:I15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1581,7 +1825,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F4" sqref="F4:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1806,21 +2050,39 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4EBB76D-5B5E-4023-A62F-5931176CF1F8}">
-  <dimension ref="A1:M15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C113E18-994F-41FE-8DC2-039E8CD107EE}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="N7" sqref="N7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4EBB76D-5B5E-4023-A62F-5931176CF1F8}">
+  <dimension ref="A1:Q15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="4" max="5" width="0" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="13.265625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
         <v>36</v>
       </c>
@@ -1845,8 +2107,14 @@
       <c r="M1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="P1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1868,14 +2136,26 @@
       <c r="G2" s="4">
         <v>-2.4429841464494602</v>
       </c>
+      <c r="K2" t="s">
+        <v>37</v>
+      </c>
       <c r="L2">
         <v>-1.9678551006100999</v>
       </c>
       <c r="M2" s="4">
         <v>-2.4429841464494602</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="O2" t="s">
+        <v>65</v>
+      </c>
+      <c r="P2" s="10">
+        <v>-2.4534615301768699</v>
+      </c>
+      <c r="Q2" s="10">
+        <v>-3.68092705856915</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1897,14 +2177,26 @@
       <c r="G3">
         <v>0.483515149242571</v>
       </c>
+      <c r="K3" t="s">
+        <v>38</v>
+      </c>
       <c r="L3" s="4">
         <v>1.2518889550000001</v>
       </c>
       <c r="M3">
         <v>0.483515149242571</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="O3" t="s">
+        <v>66</v>
+      </c>
+      <c r="P3" s="10">
+        <v>0.59299394024954399</v>
+      </c>
+      <c r="Q3" s="10">
+        <v>-0.30844909252825298</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -1926,14 +2218,26 @@
       <c r="G4" s="8">
         <v>6.7345078094897801E-2</v>
       </c>
+      <c r="K4" s="7" t="s">
+        <v>39</v>
+      </c>
       <c r="L4" s="7">
         <v>0.98850347383195303</v>
       </c>
       <c r="M4" s="8">
         <v>6.7345078094897801E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="O4" t="s">
+        <v>67</v>
+      </c>
+      <c r="P4" s="10">
+        <v>1.2518889550000001</v>
+      </c>
+      <c r="Q4" s="10">
+        <v>0.483515149242571</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -1955,14 +2259,26 @@
       <c r="G5">
         <v>0.88851962361918602</v>
       </c>
+      <c r="K5" t="s">
+        <v>40</v>
+      </c>
       <c r="L5" s="5">
         <v>1.3429980956844401</v>
       </c>
       <c r="M5">
         <v>0.88851962361918602</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="O5" t="s">
+        <v>68</v>
+      </c>
+      <c r="P5" s="10">
+        <v>0.98850347383195303</v>
+      </c>
+      <c r="Q5" s="10">
+        <v>6.7345078094897801E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -1984,14 +2300,26 @@
       <c r="G6" s="8">
         <v>-0.30844909252825298</v>
       </c>
+      <c r="K6" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="L6" s="7">
         <v>0.59299394024954399</v>
       </c>
       <c r="M6" s="8">
         <v>-0.30844909252825298</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="O6" t="s">
+        <v>69</v>
+      </c>
+      <c r="P6" s="10">
+        <v>-0.70309405732920205</v>
+      </c>
+      <c r="Q6" s="10">
+        <v>-1.7085964610406701</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -2013,14 +2341,26 @@
       <c r="G7" s="4">
         <v>2.87781954564552</v>
       </c>
+      <c r="K7" t="s">
+        <v>42</v>
+      </c>
       <c r="L7" s="4">
         <v>1.9112571375349501</v>
       </c>
       <c r="M7" s="4">
         <v>2.87781954564552</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="O7" t="s">
+        <v>70</v>
+      </c>
+      <c r="P7" s="10">
+        <v>-3.41642502437427</v>
+      </c>
+      <c r="Q7" s="10">
+        <v>-2.3047507992994101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -2042,14 +2382,26 @@
       <c r="G8" s="4">
         <v>4.1126829928413704</v>
       </c>
+      <c r="K8" t="s">
+        <v>43</v>
+      </c>
       <c r="L8" s="4">
         <v>3.9545185736600899</v>
       </c>
       <c r="M8" s="4">
         <v>4.1126829928413704</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="O8" t="s">
+        <v>71</v>
+      </c>
+      <c r="P8" s="10">
+        <v>-6.0323157697491201</v>
+      </c>
+      <c r="Q8" s="10">
+        <v>-4.4618657268891297</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -2071,14 +2423,26 @@
       <c r="G9" s="4">
         <v>-4.4618657268891297</v>
       </c>
+      <c r="K9" t="s">
+        <v>44</v>
+      </c>
       <c r="L9" s="4">
         <v>-6.0323157697491201</v>
       </c>
       <c r="M9" s="4">
         <v>-4.4618657268891297</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="O9" t="s">
+        <v>72</v>
+      </c>
+      <c r="P9" s="10">
+        <v>1.9112571375349501</v>
+      </c>
+      <c r="Q9" s="10">
+        <v>2.87781954564552</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -2100,14 +2464,26 @@
       <c r="G10" s="4">
         <v>1.53727946293465</v>
       </c>
+      <c r="K10" t="s">
+        <v>45</v>
+      </c>
       <c r="L10" s="4">
         <v>1.4120546407374099</v>
       </c>
       <c r="M10" s="4">
         <v>1.53727946293465</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="O10" t="s">
+        <v>78</v>
+      </c>
+      <c r="P10" s="10">
+        <v>-1.9678551006100999</v>
+      </c>
+      <c r="Q10" s="10">
+        <v>-2.4429841464494602</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -2132,14 +2508,26 @@
       <c r="H11" t="s">
         <v>56</v>
       </c>
+      <c r="K11" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="L11" s="7">
         <v>-0.70309405732920205</v>
       </c>
       <c r="M11" s="4">
         <v>-1.7085964610406701</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="O11" t="s">
+        <v>73</v>
+      </c>
+      <c r="P11" s="10">
+        <v>1.4120546407374099</v>
+      </c>
+      <c r="Q11" s="10">
+        <v>1.53727946293465</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -2161,14 +2549,26 @@
       <c r="G12" s="4">
         <v>-3.68092705856915</v>
       </c>
+      <c r="K12" t="s">
+        <v>47</v>
+      </c>
       <c r="L12" s="4">
         <v>-2.4534615301768699</v>
       </c>
       <c r="M12" s="4">
         <v>-3.68092705856915</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="O12" t="s">
+        <v>74</v>
+      </c>
+      <c r="P12" s="10">
+        <v>3.9545185736600899</v>
+      </c>
+      <c r="Q12" s="10">
+        <v>4.1126829928413704</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -2190,14 +2590,26 @@
       <c r="G13" s="4">
         <v>-2.0800870027327201</v>
       </c>
+      <c r="K13" t="s">
+        <v>48</v>
+      </c>
       <c r="L13" s="4">
         <v>-2.80207706491186</v>
       </c>
       <c r="M13" s="4">
         <v>-2.0800870027327201</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="O13" t="s">
+        <v>75</v>
+      </c>
+      <c r="P13" s="10">
+        <v>-2.80207706491186</v>
+      </c>
+      <c r="Q13" s="10">
+        <v>-2.0800870027327201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -2219,14 +2631,26 @@
       <c r="G14" s="4">
         <v>-2.7340215562766699</v>
       </c>
+      <c r="K14" t="s">
+        <v>49</v>
+      </c>
       <c r="L14" s="4">
         <v>-3.22091209978419</v>
       </c>
       <c r="M14" s="4">
         <v>-2.7340215562766699</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="O14" t="s">
+        <v>76</v>
+      </c>
+      <c r="P14" s="10">
+        <v>-3.22091209978419</v>
+      </c>
+      <c r="Q14" s="10">
+        <v>-2.7340215562766699</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -2248,11 +2672,23 @@
       <c r="G15" s="4">
         <v>-2.3047507992994101</v>
       </c>
+      <c r="K15" t="s">
+        <v>50</v>
+      </c>
       <c r="L15" s="4">
         <v>-3.41642502437427</v>
       </c>
       <c r="M15" s="4">
         <v>-2.3047507992994101</v>
+      </c>
+      <c r="O15" t="s">
+        <v>77</v>
+      </c>
+      <c r="P15" s="10">
+        <v>1.3429980956844401</v>
+      </c>
+      <c r="Q15" s="10">
+        <v>0.88851962361918602</v>
       </c>
     </row>
   </sheetData>
@@ -2263,12 +2699,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A818B781-5BD8-450D-A954-4A91DC498013}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -2279,711 +2715,714 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
-        <v>37</v>
+        <v>78</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="F1" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="G1" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="H1" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="I1" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="J1" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="K1" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L1" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="M1" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="N1" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="O1" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2">
+        <v>78</v>
+      </c>
+      <c r="B2" s="11">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="11">
         <v>0.83776908873656697</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="11">
         <v>0.88923915787372598</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="11">
         <v>0.117470761935885</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="11">
         <v>0.83126685634361597</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="11">
         <v>-0.72810607951055895</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="11">
         <v>-0.71946919898088901</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="11">
         <v>-0.13765567505201501</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="11">
         <v>-0.76944432540712804</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="11">
         <v>0.41685807607808101</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="11">
         <v>0.71834680784164895</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="11">
         <v>-0.27680833139310301</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="11">
         <v>0.14441799381325901</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="11">
         <v>-0.27999473956124898</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3">
+        <v>67</v>
+      </c>
+      <c r="B3" s="11">
         <v>0.83776908873656697</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="11">
         <v>1</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="11">
         <v>0.89060864151247499</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="11">
         <v>1.79384134579233E-2</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="11">
         <v>0.76971684657911998</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="11">
         <v>-0.73599582114708695</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="11">
         <v>-0.72947218104050604</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="11">
         <v>-0.28706710388066697</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="11">
         <v>-0.73933599843360898</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="11">
         <v>0.21689987793093499</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="11">
         <v>0.49741186083328098</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="11">
         <v>-0.24775437970651101</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="11">
         <v>0.113610033859759</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="11">
         <v>-0.44089875610423501</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4">
+        <v>68</v>
+      </c>
+      <c r="B4" s="11">
         <v>0.88923915787372598</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="11">
         <v>0.89060864151247499</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="11">
         <v>1</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="11">
         <v>0.13376214147099499</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="11">
         <v>0.86725762430301501</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="11">
         <v>-0.74570563487997299</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="11">
         <v>-0.71202788197807998</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="11">
         <v>-0.319254563098402</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="11">
         <v>-0.75005417645886796</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="11">
         <v>0.449209584348775</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="11">
         <v>0.67031636950235995</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="11">
         <v>-0.380392682981743</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="11">
         <v>1.0590092783407899E-3</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="11">
         <v>-0.42242812650596601</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5">
+        <v>77</v>
+      </c>
+      <c r="B5" s="11">
         <v>0.117470761935885</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="11">
         <v>1.79384134579233E-2</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="11">
         <v>0.13376214147099499</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="11">
         <v>1</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="11">
         <v>0.114397537452209</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="11">
         <v>2.5204261031728702E-2</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="11">
         <v>-7.6450117836369498E-3</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="11">
         <v>0.15376634407467299</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="11">
         <v>-0.13185168301877501</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="11">
         <v>0.222291609960486</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="11">
         <v>0.21106903450188699</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="11">
         <v>-0.314427061084677</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="11">
         <v>-6.2039656163527503E-2</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="11">
         <v>0.10942997371797</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6">
+        <v>66</v>
+      </c>
+      <c r="B6" s="11">
         <v>0.83126685634361597</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="11">
         <v>0.76971684657911998</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="11">
         <v>0.86725762430301501</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="11">
         <v>0.114397537452209</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="11">
         <v>1</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="11">
         <v>-0.733821913675755</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="11">
         <v>-0.61257517537339901</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="11">
         <v>-0.27578686976316402</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="11">
         <v>-0.70325728296513701</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="11">
         <v>0.71724109958218796</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="11">
         <v>0.74845242079623397</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="11">
         <v>-0.39362122367897801</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="11">
         <v>5.33932274672188E-2</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="11">
         <v>-0.38713713127034199</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7">
+        <v>72</v>
+      </c>
+      <c r="B7" s="11">
         <v>-0.72810607951055895</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="11">
         <v>-0.73599582114708695</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="11">
         <v>-0.74570563487997299</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="11">
         <v>2.5204261031728702E-2</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="11">
         <v>-0.733821913675755</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="11">
         <v>1</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="11">
         <v>0.71348235516439096</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="11">
         <v>0.158674041744121</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="11">
         <v>0.63704906770104797</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="11">
         <v>-0.39835559914004898</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="11">
         <v>-0.633179630393365</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="11">
         <v>0.221825767559407</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="11">
         <v>-9.06398495394444E-2</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="11">
         <v>0.25835614586920902</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8">
+        <v>74</v>
+      </c>
+      <c r="B8" s="11">
         <v>-0.71946919898088901</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="11">
         <v>-0.72947218104050604</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="11">
         <v>-0.71202788197807998</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="11">
         <v>-7.6450117836369498E-3</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="11">
         <v>-0.61257517537339901</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="11">
         <v>0.71348235516439096</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="11">
         <v>1</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="11">
         <v>-4.9304538104989998E-2</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="11">
         <v>0.77631311389343005</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="11">
         <v>-0.117468486027323</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="11">
         <v>-0.48702827718932901</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="11">
         <v>4.5965458581052297E-2</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="11">
         <v>-0.18947908420804499</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="11">
         <v>1.89815901702814E-2</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9">
+        <v>71</v>
+      </c>
+      <c r="B9" s="11">
         <v>-0.13765567505201501</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="11">
         <v>-0.28706710388066697</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="11">
         <v>-0.319254563098402</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="11">
         <v>0.15376634407467299</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="11">
         <v>-0.27578686976316402</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="11">
         <v>0.158674041744121</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="11">
         <v>-4.9304538104989998E-2</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="11">
         <v>1</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="11">
         <v>0.15007401340486301</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="11">
         <v>-0.20873384423292199</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="11">
         <v>-4.4431281907954798E-2</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="11">
         <v>0.28185483710312798</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="11">
         <v>0.40952913505359301</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="11">
         <v>0.86632391465569003</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10">
+        <v>73</v>
+      </c>
+      <c r="B10" s="11">
         <v>-0.76944432540712804</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="11">
         <v>-0.73933599843360898</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="11">
         <v>-0.75005417645886796</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="11">
         <v>-0.13185168301877501</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="11">
         <v>-0.70325728296513701</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="11">
         <v>0.63704906770104797</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="11">
         <v>0.77631311389343005</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="11">
         <v>0.15007401340486301</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="11">
         <v>1</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="11">
         <v>-0.318867413964324</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="11">
         <v>-0.57741538418399896</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="11">
         <v>0.17433471974533599</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="11">
         <v>-8.4948674175215594E-2</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="11">
         <v>0.22630837078793001</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11">
+        <v>69</v>
+      </c>
+      <c r="B11" s="11">
         <v>0.41685807607808101</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="11">
         <v>0.21689987793093499</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="11">
         <v>0.449209584348775</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="11">
         <v>0.222291609960486</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="11">
         <v>0.71724109958218796</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="11">
         <v>-0.39835559914004898</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="11">
         <v>-0.117468486027323</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="11">
         <v>-0.20873384423292199</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="11">
         <v>-0.318867413964324</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="11">
         <v>1</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="11">
         <v>0.73625261837870104</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="11">
         <v>-0.41229331768476402</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="11">
         <v>-3.5279546932909599E-2</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="11">
         <v>-0.239548385784142</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12">
+        <v>65</v>
+      </c>
+      <c r="B12" s="11">
         <v>0.71834680784164895</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="11">
         <v>0.49741186083328098</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="11">
         <v>0.67031636950235995</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="11">
         <v>0.21106903450188699</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="11">
         <v>0.74845242079623397</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="11">
         <v>-0.633179630393365</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="11">
         <v>-0.48702827718933001</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="11">
         <v>-4.4431281907954798E-2</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="11">
         <v>-0.57741538418399896</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="11">
         <v>0.73625261837870104</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="11">
         <v>1</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="11">
         <v>-0.41624143171878603</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="11">
         <v>3.4071570727826198E-3</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="11">
         <v>-0.142331885125736</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13">
+        <v>75</v>
+      </c>
+      <c r="B13" s="11">
         <v>-0.27680833139310301</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="11">
         <v>-0.24775437970651101</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="11">
         <v>-0.380392682981743</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="11">
         <v>-0.314427061084677</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="11">
         <v>-0.39362122367897801</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="11">
         <v>0.221825767559407</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="11">
         <v>4.5965458581052297E-2</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="11">
         <v>0.28185483710312798</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="11">
         <v>0.17433471974533599</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="11">
         <v>-0.41229331768476402</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="11">
         <v>-0.41624143171878603</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="11">
         <v>1</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="11">
         <v>0.63696750912630595</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="11">
         <v>0.30782499877945102</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14">
+        <v>76</v>
+      </c>
+      <c r="B14" s="11">
         <v>0.14441799381325901</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="11">
         <v>0.113610033859759</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="11">
         <v>1.0590092783407899E-3</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="11">
         <v>-6.2039656163527503E-2</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="11">
         <v>5.33932274672188E-2</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="11">
         <v>-9.06398495394444E-2</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="11">
         <v>-0.18947908420804499</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="11">
         <v>0.40952913505359301</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="11">
         <v>-8.4948674175215594E-2</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="11">
         <v>-3.5279546932909599E-2</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="11">
         <v>3.4071570727826198E-3</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="11">
         <v>0.63696750912630595</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="11">
         <v>1</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="11">
         <v>0.31994114456002698</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15">
+        <v>70</v>
+      </c>
+      <c r="B15" s="11">
         <v>-0.27999473956124898</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="11">
         <v>-0.44089875610423501</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="11">
         <v>-0.42242812650596601</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="11">
         <v>0.10942997371797</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="11">
         <v>-0.38713713127034199</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="11">
         <v>0.25835614586920902</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="11">
         <v>1.89815901702814E-2</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="11">
         <v>0.86632391465569003</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="11">
         <v>0.22630837078793001</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="11">
         <v>-0.239548385784142</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="11">
         <v>-0.142331885125736</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="11">
         <v>0.30782499877945102</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="11">
         <v>0.31994114456002698</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="11">
         <v>0.999999999999999</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B2:O15">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>0.6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>-0.8</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>